<commit_message>
Data source modification in "cotisations_TousRegimes"
</commit_message>
<xml_diff>
--- a/src/countries/france/data/sources/cotisations_TousRegimes.xlsx
+++ b/src/countries/france/data/sources/cotisations_TousRegimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="27315" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15690" windowHeight="12945"/>
   </bookViews>
   <sheets>
     <sheet name="amounts" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="sources" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1:J41"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>Maladie</t>
   </si>
@@ -155,6 +156,12 @@
   </si>
   <si>
     <t>var</t>
+  </si>
+  <si>
+    <t>cotsoc_noncontrib</t>
+  </si>
+  <si>
+    <t>cotsoc_contrib</t>
   </si>
 </sst>
 </file>
@@ -725,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +883,64 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3">
+        <v>92806000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>95002000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>97978000000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>101486000000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>104001000000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>108053000000</v>
+      </c>
+      <c r="H8" s="3">
+        <v>108818000000</v>
+      </c>
+      <c r="I8" s="3">
+        <v>110926000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3">
+        <v>89157000000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>92100000000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>94188000000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>98386000000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>102167000000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>104647000000</v>
+      </c>
+      <c r="H9" s="3">
+        <v>105452000000</v>
+      </c>
+      <c r="I9" s="3">
+        <v>112923000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -883,10 +948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1100,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>44</v>
       </c>
@@ -1064,1553 +1129,1627 @@
         <v>15651000000</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="9" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B15+B17</f>
+        <v>92806000000</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ref="C9:I9" si="0">C15+C17</f>
+        <v>95002000000</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>97978000000</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>101486000000</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>104001000000</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>108053000000</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>108818000000</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>110926000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B16+B18</f>
+        <v>89157000000</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:I10" si="1">C16+C18</f>
+        <v>92100000000</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>94188000000</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>98386000000</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>102167000000</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="1"/>
+        <v>104647000000</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>105452000000</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>112923000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2">
+    <row r="14" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
         <v>2003</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C14" s="2">
         <v>2004</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D14" s="2">
         <v>2005</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E14" s="2">
         <v>2006</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F14" s="2">
         <v>2007</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G14" s="2">
         <v>2008</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H14" s="2">
         <v>2009</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I14" s="2">
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B15" s="5">
         <v>64780000000</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C15" s="5">
         <v>66383000000</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D15" s="5">
         <v>68400000000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E15" s="5">
         <v>70774000000</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F15" s="5">
         <v>73291000000</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G15" s="5">
         <v>75199000000</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H15" s="5">
         <v>75712000000</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I15" s="5">
         <v>77251000000</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="J15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B16" s="5">
         <v>81702000000</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C16" s="5">
         <v>84488000000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D16" s="5">
         <v>86407000000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E16" s="5">
         <v>90198000000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F16" s="5">
         <v>93723000000</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G16" s="5">
         <v>95582000000</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H16" s="5">
         <v>96510000000</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I16" s="5">
         <v>103804000000</v>
       </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B17" s="5">
         <v>28026000000</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C17" s="5">
         <v>28619000000</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D17" s="5">
         <v>29578000000</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E17" s="5">
         <v>30712000000</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F17" s="5">
         <v>30710000000</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G17" s="5">
         <v>32854000000</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H17" s="5">
         <v>33106000000</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I17" s="5">
         <v>33675000000</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="18" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B18" s="5">
         <v>7455000000</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C18" s="5">
         <v>7612000000</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D18" s="5">
         <v>7781000000</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E18" s="5">
         <v>8188000000</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F18" s="5">
         <v>8444000000</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G18" s="5">
         <v>9065000000</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H18" s="5">
         <v>8942000000</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I18" s="5">
         <v>9119000000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="19" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+    </row>
+    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2">
+    <row r="24" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2">
         <v>2003</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C24" s="2">
         <v>2004</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D24" s="2">
         <v>2005</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E24" s="2">
         <v>2006</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F24" s="2">
         <v>2007</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G24" s="2">
         <v>2008</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H24" s="2">
         <v>2009</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I24" s="2">
         <v>2010</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="25" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B25" s="5">
         <v>181963000000</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C25" s="5">
         <v>187102000000</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D25" s="5">
         <v>192166000000</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E25" s="5">
         <v>199871000000</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F25" s="5">
         <v>207167000000</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G25" s="5">
         <v>212700000000</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H25" s="5">
         <v>214270000000</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I25" s="5">
         <v>223848000000</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="26" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B26" s="10">
         <v>179888000000</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C26" s="10">
         <v>184976000000</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D26" s="10">
         <v>189866000000</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E26" s="10">
         <v>197486000000</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F26" s="10">
         <v>204677000000</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G26" s="10">
         <v>210419000000</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H26" s="10">
         <v>211838000000</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I26" s="10">
         <v>221297000000</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="27" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B27" s="3">
         <v>167924000000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C27" s="3">
         <v>172964000000</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D27" s="3">
         <v>177309000000</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E27" s="3">
         <v>184041000000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F27" s="3">
         <v>190554000000</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G27" s="3">
         <v>194737000000</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H27" s="3">
         <v>195843000000</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I27" s="3">
         <v>205646000000</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="28" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B28" s="3">
         <v>132394000000</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C28" s="3">
         <v>136315000000</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D28" s="3">
         <v>139395000000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E28" s="3">
         <v>144396000000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F28" s="3">
         <v>149578000000</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G28" s="3">
         <v>154298000000</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H28" s="3">
         <v>155224000000</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I28" s="3">
         <v>164437000000</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="29" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B29" s="3">
         <v>35530000000</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C29" s="3">
         <v>36648000000</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D29" s="3">
         <v>37913000000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E29" s="3">
         <v>39645000000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F29" s="3">
         <v>40975000000</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G29" s="3">
         <v>40439000000</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H29" s="3">
         <v>40619000000</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I29" s="3">
         <v>41209000000</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+    <row r="30" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B30" s="3">
         <v>11964000000</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C30" s="3">
         <v>12013000000</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D30" s="3">
         <v>12558000000</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E30" s="3">
         <v>13445000000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F30" s="3">
         <v>14123000000</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G30" s="3">
         <v>15682000000</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H30" s="3">
         <v>15995000000</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I30" s="3">
         <v>15651000000</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="31" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B31" s="10">
         <v>658000000</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C31" s="10">
         <v>682000000</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D31" s="10">
         <v>691000000</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E31" s="10">
         <v>724000000</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F31" s="10">
         <v>687000000</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G31" s="10">
         <v>783000000</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H31" s="10">
         <v>811000000</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I31" s="10">
         <v>845000000</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+    <row r="32" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B32" s="10">
         <v>791000000</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C32" s="10">
         <v>853000000</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D32" s="10">
         <v>991000000</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E32" s="10">
         <v>1002000000</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F32" s="10">
         <v>1130000000</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G32" s="10">
         <v>1016000000</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H32" s="10">
         <v>986000000</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I32" s="10">
         <v>1049000000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="33" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B33" s="10">
         <v>627000000</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C33" s="10">
         <v>591000000</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D33" s="10">
         <v>618000000</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E33" s="10">
         <v>659000000</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F33" s="10">
         <v>673000000</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G33" s="10">
         <v>481000000</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H33" s="10">
         <v>635000000</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I33" s="10">
         <v>657000000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B35" s="5">
         <v>143766000000</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C35" s="5">
         <v>147764000000</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D35" s="5">
         <v>152221000000</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E35" s="5">
         <v>158630000000</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F35" s="5">
         <v>164294000000</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G35" s="5">
         <v>168297000000</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H35" s="5">
         <v>168966000000</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I35" s="5">
         <v>172607000000</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="36" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B36" s="10">
         <v>142291000000</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C36" s="10">
         <v>146205000000</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D36" s="10">
         <v>150586000000</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E36" s="10">
         <v>156923000000</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F36" s="10">
         <v>162440000000</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G36" s="10">
         <v>166517000000</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H36" s="10">
         <v>167022000000</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I36" s="10">
         <v>170668000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+    <row r="37" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B37" s="3">
         <v>139042000000</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C37" s="3">
         <v>143031000000</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D37" s="3">
         <v>147232000000</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E37" s="3">
         <v>153308000000</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F37" s="3">
         <v>158570000000</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G37" s="3">
         <v>162219000000</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H37" s="3">
         <v>162437000000</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I37" s="3">
         <v>166366000000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+    <row r="38" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B38" s="3">
         <v>113285000000</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C38" s="3">
         <v>116491000000</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D38" s="3">
         <v>119946000000</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E38" s="3">
         <v>124462000000</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F38" s="3">
         <v>128506000000</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G38" s="3">
         <v>132703000000</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H38" s="3">
         <v>132903000000</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I38" s="3">
         <v>136349000000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+    <row r="39" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B39" s="3">
         <v>25757000000</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C39" s="3">
         <v>26540000000</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D39" s="3">
         <v>27286000000</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E39" s="3">
         <v>28846000000</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F39" s="3">
         <v>30064000000</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G39" s="3">
         <v>29517000000</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H39" s="3">
         <v>29534000000</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I39" s="3">
         <v>30017000000</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+    <row r="40" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B40" s="3">
         <v>3249000000</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C40" s="3">
         <v>3174000000</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D40" s="3">
         <v>3354000000</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E40" s="3">
         <v>3616000000</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F40" s="3">
         <v>3869000000</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G40" s="3">
         <v>4298000000</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H40" s="3">
         <v>4585000000</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I40" s="3">
         <v>4302000000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="41" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B41" s="10">
         <v>440000000</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C41" s="10">
         <v>461000000</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D41" s="10">
         <v>456000000</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E41" s="10">
         <v>503000000</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F41" s="10">
         <v>524000000</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G41" s="10">
         <v>709000000</v>
       </c>
-      <c r="H39" s="10">
+      <c r="H41" s="10">
         <v>733000000</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I41" s="10">
         <v>766000000</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+    <row r="42" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B42" s="10">
         <v>547000000</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C42" s="10">
         <v>627000000</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D42" s="10">
         <v>712000000</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E42" s="10">
         <v>687000000</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F42" s="10">
         <v>817000000</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G42" s="10">
         <v>724000000</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H42" s="10">
         <v>730000000</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I42" s="10">
         <v>705000000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="43" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B43" s="10">
         <v>488000000</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C43" s="10">
         <v>471000000</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D43" s="10">
         <v>468000000</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E43" s="10">
         <v>517000000</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F43" s="10">
         <v>514000000</v>
       </c>
-      <c r="G41" s="10">
+      <c r="G43" s="10">
         <v>347000000</v>
       </c>
-      <c r="H41" s="10">
+      <c r="H43" s="10">
         <v>481000000</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I43" s="10">
         <v>468000000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B45" s="5">
         <v>5933000000</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C45" s="5">
         <v>6065000000</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D45" s="5">
         <v>6298000000</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E45" s="5">
         <v>6255000000</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F45" s="5">
         <v>6260000000</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G45" s="5">
         <v>6333000000</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H45" s="5">
         <v>6528000000</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I45" s="5">
         <v>6290000000</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="46" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B46" s="10">
         <v>5879000000</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C46" s="10">
         <v>5991000000</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D46" s="10">
         <v>6201000000</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E46" s="10">
         <v>6133000000</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F46" s="10">
         <v>6146000000</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G46" s="10">
         <v>6227000000</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H46" s="10">
         <v>6429000000</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I46" s="10">
         <v>6194000000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="47" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B47" s="3">
         <v>3871000000</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C47" s="3">
         <v>3993000000</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D47" s="3">
         <v>4151000000</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E47" s="3">
         <v>4195000000</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F47" s="3">
         <v>4257000000</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G47" s="3">
         <v>4202000000</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H47" s="3">
         <v>4307000000</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I47" s="3">
         <v>4277000000</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="48" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B48" s="3">
         <v>2910000000</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C48" s="3">
         <v>2932000000</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D48" s="3">
         <v>3040000000</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E48" s="3">
         <v>3039000000</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F48" s="3">
         <v>3079000000</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G48" s="3">
         <v>3125000000</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H48" s="3">
         <v>3214000000</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I48" s="3">
         <v>3182000000</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="49" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B49" s="3">
         <v>961000000</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C49" s="3">
         <v>1061000000</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D49" s="3">
         <v>1112000000</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E49" s="3">
         <v>1156000000</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F49" s="3">
         <v>1178000000</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G49" s="3">
         <v>1077000000</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H49" s="3">
         <v>1093000000</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I49" s="3">
         <v>1095000000</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+    <row r="50" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B50" s="3">
         <v>2009000000</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C50" s="3">
         <v>1999000000</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D50" s="3">
         <v>2050000000</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E50" s="3">
         <v>1938000000</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F50" s="3">
         <v>1889000000</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G50" s="3">
         <v>2025000000</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H50" s="3">
         <v>2122000000</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I50" s="3">
         <v>1917000000</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="51" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B51" s="10">
         <v>0</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C51" s="10">
         <v>18000000</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D51" s="10">
         <v>17000000</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E51" s="10">
         <v>13000000</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F51" s="10">
         <v>16000000</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G51" s="10">
         <v>18000000</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H51" s="10">
         <v>19000000</v>
       </c>
-      <c r="I49" s="10">
+      <c r="I51" s="10">
         <v>19000000</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+    <row r="52" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B52" s="10">
         <v>7000000</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C52" s="10">
         <v>1000000</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D52" s="10">
         <v>29000000</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E52" s="10">
         <v>53000000</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F52" s="10">
         <v>48000000</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G52" s="10">
         <v>45000000</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H52" s="10">
         <v>37000000</v>
       </c>
-      <c r="I50" s="10">
+      <c r="I52" s="10">
         <v>31000000</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="53" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B53" s="10">
         <v>46000000</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C53" s="10">
         <v>54000000</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D53" s="10">
         <v>51000000</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E53" s="10">
         <v>56000000</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F53" s="10">
         <v>50000000</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G53" s="10">
         <v>44000000</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H53" s="10">
         <v>43000000</v>
       </c>
-      <c r="I51" s="10">
+      <c r="I53" s="10">
         <v>46000000</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+    </row>
+    <row r="55" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B55" s="5">
         <v>25401000000</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C55" s="5">
         <v>26350000000</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D55" s="5">
         <v>28385000000</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E55" s="5">
         <v>26983000000</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F55" s="5">
         <v>28126000000</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G55" s="5">
         <v>28608900000</v>
       </c>
-      <c r="H53" s="5">
+      <c r="H55" s="5">
         <v>29367800000</v>
       </c>
-      <c r="I53" s="5">
+      <c r="I55" s="5">
         <v>35365000000</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="56" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B56" s="10">
         <v>25004000000</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C56" s="10">
         <v>25932000000</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D56" s="10">
         <v>25918000000</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E56" s="10">
         <v>26529000000</v>
       </c>
-      <c r="F54" s="10">
+      <c r="F56" s="10">
         <v>27719000000</v>
       </c>
-      <c r="G54" s="10">
+      <c r="G56" s="10">
         <v>28307000000</v>
       </c>
-      <c r="H54" s="10">
+      <c r="H56" s="10">
         <v>29090000000</v>
       </c>
-      <c r="I54" s="10">
+      <c r="I56" s="10">
         <v>34994000000</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+    <row r="57" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B57" s="15">
         <v>25004000000</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C57" s="3">
         <v>25932000000</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D57" s="3">
         <v>25918000000</v>
       </c>
-      <c r="E55" s="22">
+      <c r="E57" s="22">
         <v>26529000000</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F57" s="3">
         <v>27718000000</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G57" s="3">
         <v>28307000000</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H57" s="3">
         <v>29090000000</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I57" s="3">
         <v>34993000000</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="58" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B58" s="15">
         <v>16192000000</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C58" s="3">
         <v>16885000000</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D58" s="3">
         <v>16402000000</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E58" s="3">
         <v>16886000000</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F58" s="3">
         <v>17985000000</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G58" s="3">
         <v>18462000000</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H58" s="3">
         <v>19098000000</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I58" s="3">
         <v>24896000000</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+    <row r="59" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B59" s="3">
         <v>8812000000</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C59" s="3">
         <v>9047000000</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D59" s="3">
         <v>9516000000</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E59" s="3">
         <v>9643000000</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F59" s="3">
         <v>9733000000</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G59" s="3">
         <v>9845000000</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H59" s="3">
         <v>9992000000</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I59" s="3">
         <v>10097000000</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+    <row r="60" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="19">
+      <c r="B60" s="19">
         <v>0</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C60" s="3">
         <v>0</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D60" s="3">
         <v>0</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E60" s="3">
         <v>0</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F60" s="3">
         <v>0</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G60" s="3">
         <v>0</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H60" s="3">
         <v>0</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I60" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="61" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B61" s="10">
         <v>201000000</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C61" s="10">
         <v>203000000</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D61" s="10">
         <v>218000000</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E61" s="10">
         <v>208000000</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F61" s="10">
         <v>147000000</v>
       </c>
-      <c r="G59" s="10">
+      <c r="G61" s="10">
         <v>56000000</v>
       </c>
-      <c r="H59" s="10">
+      <c r="H61" s="10">
         <v>59000000</v>
       </c>
-      <c r="I59" s="10">
+      <c r="I61" s="10">
         <v>59000000</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="62" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B62" s="10">
         <v>185000000</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C62" s="10">
         <v>206000000</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D62" s="10">
         <v>230000000</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E62" s="10">
         <v>241000000</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F62" s="10">
         <v>251000000</v>
       </c>
-      <c r="G60" s="10">
+      <c r="G62" s="10">
         <v>237000000</v>
       </c>
-      <c r="H60" s="10">
+      <c r="H62" s="10">
         <v>209000000</v>
       </c>
-      <c r="I60" s="10">
+      <c r="I62" s="10">
         <v>304000000</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="63" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B63" s="10">
         <v>11000000</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C63" s="10">
         <v>8000000</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D63" s="10">
         <v>19000000</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E63" s="10">
         <v>5000000</v>
       </c>
-      <c r="F61" s="10">
+      <c r="F63" s="10">
         <v>8000000</v>
       </c>
-      <c r="G61" s="10">
+      <c r="G63" s="10">
         <v>10000000</v>
       </c>
-      <c r="H61" s="10">
+      <c r="H63" s="10">
         <v>10000000</v>
       </c>
-      <c r="I61" s="10">
+      <c r="I63" s="10">
         <v>8000000</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="64" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B65" s="5">
         <v>6848000000</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C65" s="5">
         <v>6924000000</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D65" s="5">
         <v>7261000000</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E65" s="5">
         <v>8003000000</v>
       </c>
-      <c r="F63" s="5">
+      <c r="F65" s="5">
         <v>8488000000</v>
       </c>
-      <c r="G63" s="5">
+      <c r="G65" s="5">
         <v>9458900000</v>
       </c>
-      <c r="H63" s="5">
+      <c r="H65" s="5">
         <v>9408700000</v>
       </c>
-      <c r="I63" s="5">
+      <c r="I65" s="5">
         <v>9586000000</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+    <row r="66" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B66" s="10">
         <v>6714000000</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C66" s="10">
         <v>6848000000</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D66" s="10">
         <v>7161000000</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E66" s="10">
         <v>7900000000</v>
       </c>
-      <c r="F64" s="10">
+      <c r="F66" s="10">
         <v>8372000000</v>
       </c>
-      <c r="G64" s="10">
+      <c r="G66" s="10">
         <v>9367000000</v>
       </c>
-      <c r="H64" s="10">
+      <c r="H66" s="10">
         <v>9297000000</v>
       </c>
-      <c r="I64" s="10">
+      <c r="I66" s="10">
         <v>9441000000</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+    <row r="67" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B67" s="15">
         <v>8000000</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C67" s="3">
         <v>8000000</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D67" s="3">
         <v>7000000</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E67" s="3">
         <v>9000000</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F67" s="3">
         <v>8000000</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G67" s="3">
         <v>9000000</v>
       </c>
-      <c r="H65" s="3">
+      <c r="H67" s="3">
         <v>9000000</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I67" s="3">
         <v>10000000</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+    <row r="68" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B68" s="15">
         <v>8000000</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C68" s="3">
         <v>8000000</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D68" s="3">
         <v>7000000</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E68" s="3">
         <v>9000000</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F68" s="3">
         <v>8000000</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G68" s="3">
         <v>9000000</v>
       </c>
-      <c r="H66" s="3">
+      <c r="H68" s="3">
         <v>9000000</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I68" s="3">
         <v>10000000</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
+    <row r="69" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B69" s="3">
         <v>0</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C69" s="3">
         <v>0</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D69" s="3">
         <v>0</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E69" s="3">
         <v>0</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F69" s="3">
         <v>0</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G69" s="3">
         <v>0</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H69" s="3">
         <v>0</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I69" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+    <row r="70" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B70" s="3">
         <v>6706000000</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C70" s="3">
         <v>6840000000</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D70" s="3">
         <v>7154000000</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E70" s="3">
         <v>7892000000</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F70" s="3">
         <v>8364000000</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G70" s="3">
         <v>9358000000</v>
       </c>
-      <c r="H68" s="3">
+      <c r="H70" s="3">
         <v>9288000000</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I70" s="3">
         <v>9431000000</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+    <row r="71" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B71" s="10">
         <v>0</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C71" s="10">
         <v>0</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D71" s="10">
         <v>0</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E71" s="10">
         <v>0</v>
       </c>
-      <c r="F69" s="10">
+      <c r="F71" s="10">
         <v>0</v>
       </c>
-      <c r="G69" s="10">
+      <c r="G71" s="10">
         <v>0</v>
       </c>
-      <c r="H69" s="10">
+      <c r="H71" s="10">
         <v>0</v>
       </c>
-      <c r="I69" s="10">
+      <c r="I71" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+    <row r="72" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B72" s="10">
         <v>53000000</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C72" s="10">
         <v>18000000</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D72" s="10">
         <v>20000000</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E72" s="10">
         <v>21000000</v>
       </c>
-      <c r="F70" s="10">
+      <c r="F72" s="10">
         <v>14000000</v>
       </c>
-      <c r="G70" s="10">
+      <c r="G72" s="10">
         <v>11000000</v>
       </c>
-      <c r="H70" s="10">
+      <c r="H72" s="10">
         <v>10000000</v>
       </c>
-      <c r="I70" s="10">
+      <c r="I72" s="10">
         <v>9000000</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+    <row r="73" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B71" s="10">
+      <c r="B73" s="10">
         <v>81000000</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C73" s="10">
         <v>58000000</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D73" s="10">
         <v>80000000</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E73" s="10">
         <v>81000000</v>
       </c>
-      <c r="F71" s="10">
+      <c r="F73" s="10">
         <v>101000000</v>
       </c>
-      <c r="G71" s="10">
+      <c r="G73" s="10">
         <v>81000000</v>
       </c>
-      <c r="H71" s="10">
+      <c r="H73" s="10">
         <v>102000000</v>
       </c>
-      <c r="I71" s="10">
+      <c r="I73" s="10">
         <v>136000000</v>
       </c>
     </row>

</xml_diff>